<commit_message>
Update receipt recognizer PoC results xlsx to include result of date/time ingest
</commit_message>
<xml_diff>
--- a/PoCs/FormRecognizer-Receipts/poc-results.xlsx
+++ b/PoCs/FormRecognizer-Receipts/poc-results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paelaz\Code\plzm.github\azure-cognitive\PoCs\FormRecognizer-Receipts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2410A4BF-9797-45CE-A8A1-089392DFDBA9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F735529B-3AE5-45C9-87D6-65D6B0680D5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="750" windowWidth="24990" windowHeight="18180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1635" yWindow="1335" windowWidth="23670" windowHeight="18150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="191">
   <si>
     <t>ReceiptGuid</t>
   </si>
@@ -578,6 +578,21 @@
   </si>
   <si>
     <t>{"status":"Succeeded","recognitionResults":[{"page":1,"clockwiseOrientation":0.01,"width":474,"height":310,"unit":"pixel","lines":[{"boundingBox":[4,11,155,13,154,39,3,36],"text":"Veggie Fajita","words":[{"boundingBox":[6,11,82,14,82,38,5,38],"text":"Veggie"},{"boundingBox":[87,14,155,14,154,39,87,38],"text":"Fajita"}]},{"boundingBox":[426,19,473,21,473,42,425,43],"text":"6.55","words":[{"boundingBox":[428,18,472,18,472,42,427,42],"text":"6.55"}]},{"boundingBox":[3,66,140,67,139,92,2,91],"text":"Chicken Bowl","words":[{"boundingBox":[4,67,89,68,89,92,4,92],"text":"Chicken"},{"boundingBox":[96,68,140,68,140,92,96,92],"text":"Bowl","confidence":"Low"}]},{"boundingBox":[425,72,471,73,470,96,425,95],"text":"6.55","words":[{"boundingBox":[426,71,470,72,470,95,426,94],"text":"6.55"}]},{"boundingBox":[0,123,117,122,118,146,0,147],"text":"Small Soda","words":[{"boundingBox":[4,124,68,123,67,147,4,147],"text":"Small","confidence":"Low"},{"boundingBox":[72,123,118,123,117,147,72,147],"text":"Soda"}]},{"boundingBox":[424,127,471,126,471,150,424,149],"text":"1.87","words":[{"boundingBox":[427,126,470,126,470,150,427,150],"text":"1.87"}]},{"boundingBox":[2,178,92,178,92,203,2,203],"text":"Subtotal","words":[{"boundingBox":[2,178,92,178,91,203,2,204],"text":"Subtotal","confidence":"Low"}]},{"boundingBox":[412,180,468,180,467,203,412,204],"text":"14.97","words":[{"boundingBox":[414,179,467,179,467,203,415,203],"text":"14.97"}]},{"boundingBox":[0,209,37,209,36,229,0,229],"text":"Tax","words":[{"boundingBox":[2,209,36,209,36,229,2,229],"text":"Tax"}]},{"boundingBox":[424,207,468,207,467,229,424,229],"text":"1.05","words":[{"boundingBox":[425,207,466,207,466,229,425,229],"text":"1.05","confidence":"Low"}]},{"boundingBox":[1,264,58,263,58,287,2,287],"text":"Round","words":[{"boundingBox":[0,262,56,262,56,286,0,286],"text":"Round"}]},{"boundingBox":[411,260,465,259,465,283,411,282],"text":"-0.02","words":[{"boundingBox":[412,259,463,259,463,283,412,283],"text":"-0.02"}]},{"boundingBox":[0,289,147,287,148,308,0,310],"text":"DINE IN Total","words":[{"boundingBox":[0,291,44,290,45,309,0,309],"text":"DINE","confidence":"Low"},{"boundingBox":[58,290,80,289,80,309,59,309],"text":"IN","confidence":"Low"},{"boundingBox":[93,289,148,288,148,309,93,309],"text":"Total","confidence":"Low"}]},{"boundingBox":[410,285,465,286,465,309,409,309],"text":"16.00","words":[{"boundingBox":[412,284,464,284,464,308,411,308],"text":"16.00"}]}]}],"understandingResults":[{"pages":[1],"fields":{"Subtotal":{"valueType":"numberValue","value":14.97,"text":"14.97","elements":[{"$ref":"#/recognitionResults/0/lines/7/words/0"}]},"Total":{"valueType":"numberValue","value":16.0,"text":"16.00","elements":[{"$ref":"#/recognitionResults/0/lines/13/words/0"}]},"Tax":{"valueType":"numberValue","value":1.05,"text":"1.05","elements":[{"$ref":"#/recognitionResults/0/lines/9/words/0"}]},"MerchantAddress":null,"MerchantName":{"valueType":"stringValue","value":"Veggie Fajita","text":"Veggie Fajita","elements":[{"$ref":"#/recognitionResults/0/lines/0/words/0"},{"$ref":"#/recognitionResults/0/lines/0/words/1"}]},"MerchantPhoneNumber":null,"TransactionDate":null,"TransactionTime":null}}]}</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes - time only</t>
+  </si>
+  <si>
+    <t>Yes (but FR)</t>
+  </si>
+  <si>
+    <t>Receipt has date/time?</t>
   </si>
 </sst>
 </file>
@@ -587,7 +602,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -599,6 +614,22 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -625,10 +656,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -944,10 +977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,12 +994,13 @@
     <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="241.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="241.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -995,19 +1029,22 @@
         <v>9</v>
       </c>
       <c r="J1" t="s">
+        <v>190</v>
+      </c>
+      <c r="K1" t="s">
         <v>1</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1029,20 +1066,23 @@
       <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>20</v>
-      </c>
-      <c r="L2" s="1">
-        <v>43690.536611921299</v>
       </c>
       <c r="M2" s="1">
         <v>43690.536611921299</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" s="1">
+        <v>43690.536611921299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1064,20 +1104,23 @@
       <c r="G3" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>29</v>
-      </c>
-      <c r="L3" s="1">
-        <v>43690.551832060184</v>
       </c>
       <c r="M3" s="1">
         <v>43690.551832060184</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" s="1">
+        <v>43690.551832060184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1096,20 +1139,23 @@
       <c r="G4" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>35</v>
-      </c>
-      <c r="L4" s="1">
-        <v>43690.551832291669</v>
       </c>
       <c r="M4" s="1">
         <v>43690.551832291669</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" s="1">
+        <v>43690.551832291669</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1131,20 +1177,23 @@
       <c r="G5" t="s">
         <v>42</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>43</v>
-      </c>
-      <c r="L5" s="1">
-        <v>43690.551833217593</v>
       </c>
       <c r="M5" s="1">
         <v>43690.551833217593</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" s="1">
+        <v>43690.551833217593</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1163,20 +1212,23 @@
       <c r="G6" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>49</v>
-      </c>
-      <c r="L6" s="1">
-        <v>43690.551833564816</v>
       </c>
       <c r="M6" s="1">
         <v>43690.551833564816</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" s="1">
+        <v>43690.551833564816</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -1201,20 +1253,23 @@
       <c r="I7" t="s">
         <v>55</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>56</v>
-      </c>
-      <c r="L7" s="1">
-        <v>43690.55183364197</v>
       </c>
       <c r="M7" s="1">
         <v>43690.55183364197</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" s="1">
+        <v>43690.55183364197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -1236,20 +1291,23 @@
       <c r="G8" t="s">
         <v>62</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>63</v>
-      </c>
-      <c r="L8" s="1">
-        <v>43690.551833680554</v>
       </c>
       <c r="M8" s="1">
         <v>43690.551833680554</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8" s="1">
+        <v>43690.551833680554</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -1274,20 +1332,20 @@
       <c r="I9" t="s">
         <v>69</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>70</v>
-      </c>
-      <c r="L9" s="1">
-        <v>43690.551833796293</v>
       </c>
       <c r="M9" s="1">
         <v>43690.551833796293</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9" s="1">
+        <v>43690.551833796293</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>71</v>
       </c>
@@ -1309,20 +1367,20 @@
       <c r="I10" t="s">
         <v>78</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>79</v>
-      </c>
-      <c r="L10" s="1">
-        <v>43690.552470254632</v>
       </c>
       <c r="M10" s="1">
         <v>43690.552470254632</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10" s="1">
+        <v>43690.552470254632</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -1350,20 +1408,20 @@
       <c r="I11" t="s">
         <v>89</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="K11" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>90</v>
-      </c>
-      <c r="L11" s="1">
-        <v>43690.552470717594</v>
       </c>
       <c r="M11" s="1">
         <v>43690.552470717594</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11" s="1">
+        <v>43690.552470717594</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>91</v>
       </c>
@@ -1379,20 +1437,23 @@
       <c r="H12" t="s">
         <v>93</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="K12" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>94</v>
-      </c>
-      <c r="L12" s="1">
-        <v>43690.552470910494</v>
       </c>
       <c r="M12" s="1">
         <v>43690.552470910494</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12" s="1">
+        <v>43690.552470910494</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>95</v>
       </c>
@@ -1417,20 +1478,20 @@
       <c r="I13" t="s">
         <v>103</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>104</v>
-      </c>
-      <c r="L13" s="1">
-        <v>43690.552470949071</v>
       </c>
       <c r="M13" s="1">
         <v>43690.552470949071</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13" s="1">
+        <v>43690.552470949071</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>105</v>
       </c>
@@ -1458,20 +1519,20 @@
       <c r="I14" t="s">
         <v>113</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="K14" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>114</v>
-      </c>
-      <c r="L14" s="1">
-        <v>43690.551833564816</v>
       </c>
       <c r="M14" s="1">
         <v>43690.551833564816</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14" s="1">
+        <v>43690.551833564816</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>115</v>
       </c>
@@ -1499,20 +1560,20 @@
       <c r="I15" t="s">
         <v>123</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>124</v>
-      </c>
-      <c r="L15" s="1">
-        <v>43690.552470717594</v>
       </c>
       <c r="M15" s="1">
         <v>43690.552470717594</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15" s="1">
+        <v>43690.552470717594</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>125</v>
       </c>
@@ -1525,20 +1586,23 @@
       <c r="D16" t="s">
         <v>129</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="K16" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>130</v>
-      </c>
-      <c r="L16" s="1">
-        <v>43690.552477777775</v>
       </c>
       <c r="M16" s="1">
         <v>43690.552477777775</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="1">
+        <v>43690.552477777775</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>131</v>
       </c>
@@ -1566,20 +1630,20 @@
       <c r="I17" t="s">
         <v>137</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="K17" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>138</v>
-      </c>
-      <c r="L17" s="1">
-        <v>43690.552650308637</v>
       </c>
       <c r="M17" s="1">
         <v>43690.552650308637</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="1">
+        <v>43690.552650308637</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>139</v>
       </c>
@@ -1601,20 +1665,20 @@
       <c r="I18" t="s">
         <v>143</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="K18" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>144</v>
-      </c>
-      <c r="L18" s="1">
-        <v>43690.55265061729</v>
       </c>
       <c r="M18" s="1">
         <v>43690.55265061729</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="1">
+        <v>43690.55265061729</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>145</v>
       </c>
@@ -1636,20 +1700,23 @@
       <c r="G19" t="s">
         <v>151</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J19" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="K19" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>152</v>
-      </c>
-      <c r="L19" s="1">
-        <v>43690.551833834877</v>
       </c>
       <c r="M19" s="1">
         <v>43690.551833834877</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19" s="1">
+        <v>43690.551833834877</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>153</v>
       </c>
@@ -1677,20 +1744,20 @@
       <c r="I20" t="s">
         <v>162</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="K20" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>163</v>
-      </c>
-      <c r="L20" s="1">
-        <v>43690.552470100309</v>
       </c>
       <c r="M20" s="1">
         <v>43690.552470100309</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20" s="1">
+        <v>43690.552470100309</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>164</v>
       </c>
@@ -1718,20 +1785,20 @@
       <c r="I21" t="s">
         <v>172</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="K21" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>173</v>
-      </c>
-      <c r="L21" s="1">
-        <v>43690.552470408955</v>
       </c>
       <c r="M21" s="1">
         <v>43690.552470408955</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21" s="1">
+        <v>43690.552470408955</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>174</v>
       </c>
@@ -1750,20 +1817,23 @@
       <c r="I22" t="s">
         <v>177</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="J22" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="K22" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>178</v>
-      </c>
-      <c r="L22" s="1">
-        <v>43690.552471026233</v>
       </c>
       <c r="M22" s="1">
         <v>43690.552471026233</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22" s="1">
+        <v>43690.552471026233</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>179</v>
       </c>
@@ -1779,44 +1849,48 @@
       <c r="E23" t="s">
         <v>184</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="J23" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="K23" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>185</v>
-      </c>
-      <c r="L23" s="1">
-        <v>43690.552470293216</v>
       </c>
       <c r="M23" s="1">
         <v>43690.552470293216</v>
       </c>
+      <c r="N23" s="1">
+        <v>43690.552470293216</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{708F17AA-2559-4882-9AEA-40BD7A9B4E93}"/>
-    <hyperlink ref="J3" r:id="rId2" xr:uid="{F93A05F4-ECA5-4D8A-B048-D60001648F19}"/>
-    <hyperlink ref="J4" r:id="rId3" xr:uid="{4290D49A-00C4-4A55-B5E4-5840729CFC99}"/>
-    <hyperlink ref="J5" r:id="rId4" xr:uid="{BF4A5230-903B-4209-8823-5A9E5D0521E3}"/>
-    <hyperlink ref="J6" r:id="rId5" xr:uid="{16CA2AD1-F75F-4666-99C1-0A24FEB96832}"/>
-    <hyperlink ref="J7" r:id="rId6" xr:uid="{3E74912A-57D7-464C-88ED-AF72D781E6FD}"/>
-    <hyperlink ref="J8" r:id="rId7" xr:uid="{A65009D3-E8B4-4D83-AB83-A83DD18EF0CB}"/>
-    <hyperlink ref="J9" r:id="rId8" xr:uid="{7136CD40-80D9-464E-80B2-2ED664847145}"/>
-    <hyperlink ref="J11" r:id="rId9" xr:uid="{8A313355-98E0-4AAC-9B60-A9AB688D1E9F}"/>
-    <hyperlink ref="J10" r:id="rId10" xr:uid="{310184DF-5A9B-4238-9890-8A5F4F8C1E54}"/>
-    <hyperlink ref="J12" r:id="rId11" xr:uid="{53C6CB83-2CEB-4015-9531-84B5A880B0E4}"/>
-    <hyperlink ref="J13" r:id="rId12" xr:uid="{59324B93-F5F8-472C-B723-02AE2834FD17}"/>
-    <hyperlink ref="J14" r:id="rId13" xr:uid="{F5A3FE3A-9C0B-40A5-B276-626ADDA7F4FE}"/>
-    <hyperlink ref="J15" r:id="rId14" xr:uid="{17EDFD8B-862E-4400-B233-817E1E3C0E66}"/>
-    <hyperlink ref="J16" r:id="rId15" xr:uid="{564FAA33-643B-445B-AF2A-4E841DA90BD3}"/>
-    <hyperlink ref="J17" r:id="rId16" xr:uid="{1A9E0210-3C2D-4FEA-86D8-4563657CA6C5}"/>
-    <hyperlink ref="J18" r:id="rId17" xr:uid="{70B5CDB2-BC42-492C-BB84-41C7835CCF9E}"/>
-    <hyperlink ref="J19" r:id="rId18" xr:uid="{0C25B461-52D3-4076-BBB6-0139BD46771D}"/>
-    <hyperlink ref="J20" r:id="rId19" xr:uid="{CD99CE46-C9C1-40F2-80E8-5D30F16B6670}"/>
-    <hyperlink ref="J21" r:id="rId20" xr:uid="{DA560139-4C34-4168-A16A-1E71CAC8B5F9}"/>
-    <hyperlink ref="J22" r:id="rId21" xr:uid="{AAC3E90E-5D71-43E2-BFE1-EBB23641C11B}"/>
-    <hyperlink ref="J23" r:id="rId22" xr:uid="{37F423C7-0358-4F81-9AC6-E929184EFD98}"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{708F17AA-2559-4882-9AEA-40BD7A9B4E93}"/>
+    <hyperlink ref="K3" r:id="rId2" xr:uid="{F93A05F4-ECA5-4D8A-B048-D60001648F19}"/>
+    <hyperlink ref="K4" r:id="rId3" xr:uid="{4290D49A-00C4-4A55-B5E4-5840729CFC99}"/>
+    <hyperlink ref="K5" r:id="rId4" xr:uid="{BF4A5230-903B-4209-8823-5A9E5D0521E3}"/>
+    <hyperlink ref="K6" r:id="rId5" xr:uid="{16CA2AD1-F75F-4666-99C1-0A24FEB96832}"/>
+    <hyperlink ref="K7" r:id="rId6" xr:uid="{3E74912A-57D7-464C-88ED-AF72D781E6FD}"/>
+    <hyperlink ref="K8" r:id="rId7" xr:uid="{A65009D3-E8B4-4D83-AB83-A83DD18EF0CB}"/>
+    <hyperlink ref="K9" r:id="rId8" xr:uid="{7136CD40-80D9-464E-80B2-2ED664847145}"/>
+    <hyperlink ref="K11" r:id="rId9" xr:uid="{8A313355-98E0-4AAC-9B60-A9AB688D1E9F}"/>
+    <hyperlink ref="K10" r:id="rId10" xr:uid="{310184DF-5A9B-4238-9890-8A5F4F8C1E54}"/>
+    <hyperlink ref="K12" r:id="rId11" xr:uid="{53C6CB83-2CEB-4015-9531-84B5A880B0E4}"/>
+    <hyperlink ref="K13" r:id="rId12" xr:uid="{59324B93-F5F8-472C-B723-02AE2834FD17}"/>
+    <hyperlink ref="K14" r:id="rId13" xr:uid="{F5A3FE3A-9C0B-40A5-B276-626ADDA7F4FE}"/>
+    <hyperlink ref="K15" r:id="rId14" xr:uid="{17EDFD8B-862E-4400-B233-817E1E3C0E66}"/>
+    <hyperlink ref="K16" r:id="rId15" xr:uid="{564FAA33-643B-445B-AF2A-4E841DA90BD3}"/>
+    <hyperlink ref="K17" r:id="rId16" xr:uid="{1A9E0210-3C2D-4FEA-86D8-4563657CA6C5}"/>
+    <hyperlink ref="K18" r:id="rId17" xr:uid="{70B5CDB2-BC42-492C-BB84-41C7835CCF9E}"/>
+    <hyperlink ref="K19" r:id="rId18" xr:uid="{0C25B461-52D3-4076-BBB6-0139BD46771D}"/>
+    <hyperlink ref="K20" r:id="rId19" xr:uid="{CD99CE46-C9C1-40F2-80E8-5D30F16B6670}"/>
+    <hyperlink ref="K21" r:id="rId20" xr:uid="{DA560139-4C34-4168-A16A-1E71CAC8B5F9}"/>
+    <hyperlink ref="K22" r:id="rId21" xr:uid="{AAC3E90E-5D71-43E2-BFE1-EBB23641C11B}"/>
+    <hyperlink ref="K23" r:id="rId22" xr:uid="{37F423C7-0358-4F81-9AC6-E929184EFD98}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>